<commit_message>
adding a bunch of languages
</commit_message>
<xml_diff>
--- a/03_Materials/finalize_stimuli/pt/pt_br/pt_stimuli_translated_Brazilian.xlsx
+++ b/03_Materials/finalize_stimuli/pt/pt_br/pt_stimuli_translated_Brazilian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/SPAML/SPAML-PSA/03_Materials/finalize_stimuli/pt/pt_br/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AA519B-13F4-EC4E-8478-464A5833898B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C92FF2-8137-A44E-A1EC-2393CFBDC485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6483" uniqueCount="6200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6483" uniqueCount="6202">
   <si>
     <t>pt_target</t>
   </si>
@@ -18620,13 +18620,19 @@
   </si>
   <si>
     <t>cozursky</t>
+  </si>
+  <si>
+    <t>soar</t>
+  </si>
+  <si>
+    <t>sibilar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -18649,11 +18655,20 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -18682,12 +18697,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18908,8 +18924,8 @@
   </sheetPr>
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A564" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G579" sqref="G579"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D301" sqref="D301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -26335,14 +26351,14 @@
       <c r="A298" s="1" t="s">
         <v>1728</v>
       </c>
-      <c r="B298" s="1" t="s">
-        <v>173</v>
+      <c r="B298" s="4" t="s">
+        <v>6200</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>1727</v>
       </c>
-      <c r="D298" s="1" t="s">
-        <v>174</v>
+      <c r="D298" s="5" t="s">
+        <v>6201</v>
       </c>
       <c r="E298" s="1" t="s">
         <v>6140</v>

</xml_diff>